<commit_message>
🖼️ Thêm ảnh ghi chú và cập nhật nội dung
</commit_message>
<xml_diff>
--- a/Ngân hàng môn giải phẫu.xlsx
+++ b/Ngân hàng môn giải phẫu.xlsx
@@ -11170,12 +11170,18 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Khó ?</t>
+          <t>Khó ?
+![image](note_Câu 436_1750952390.png)
+![image](note_Câu 436_1750952410.png)</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Tá tụy</t>
+        </is>
+      </c>
       <c r="B23" t="inlineStr">
         <is>
           <t>Câu 437</t>
@@ -11196,10 +11202,22 @@
           <t>Module Tiêu hóa</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+![Câu A](note_Câu 437_1750952704.png)
+![Câu B → Đoạn trong thành Tá tràng mới là hẹp nhất](note_Câu 437_1750952860.png)
+![Câu C](note_Câu 437_1750952641.png)
+![Câu D](note_Câu 437_1750952500.png)</t>
+        </is>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr"/>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Tá tràng</t>
+        </is>
+      </c>
       <c r="B24" t="inlineStr">
         <is>
           <t>Câu 438</t>
@@ -11220,10 +11238,19 @@
           <t>Module Tiêu hóa</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+![image](note_Câu 438_1750952979.png)</t>
+        </is>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr"/>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Tá tràng</t>
+        </is>
+      </c>
       <c r="B25" t="inlineStr">
         <is>
           <t>Câu 439</t>
@@ -11244,10 +11271,19 @@
           <t>Module Tiêu hóa</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+![image](note_Câu 439_1750953072.png)</t>
+        </is>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr"/>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Tá tràng</t>
+        </is>
+      </c>
       <c r="B26" t="inlineStr">
         <is>
           <t>Câu 440</t>
@@ -11268,10 +11304,19 @@
           <t>Module Tiêu hóa</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+![image](note_Câu 440_1750953390.png)</t>
+        </is>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr"/>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Tụy</t>
+        </is>
+      </c>
       <c r="B27" t="inlineStr">
         <is>
           <t>Câu 441</t>
@@ -11292,10 +11337,20 @@
           <t>Module Tiêu hóa</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>![image](note_Câu 441_1750953998.png)
+![image](note_Câu 441_1750954229.png)
+![image](note_Câu 441_1750954107.png)</t>
+        </is>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Tá tràng</t>
+        </is>
+      </c>
       <c r="B28" t="inlineStr">
         <is>
           <t>Câu 442</t>
@@ -11316,10 +11371,20 @@
           <t>Module Tiêu hóa</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+![image](note_Câu 442_1750954324.png)
+![image](note_Câu 442_1750954385.png)</t>
+        </is>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr"/>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Tá tràng</t>
+        </is>
+      </c>
       <c r="B29" t="inlineStr">
         <is>
           <t>Câu 443</t>
@@ -11340,10 +11405,19 @@
           <t>Module Tiêu hóa</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+![image](note_Câu 443_1750954680.png)</t>
+        </is>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr"/>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Tá tràng</t>
+        </is>
+      </c>
       <c r="B30" t="inlineStr">
         <is>
           <t>Câu 444</t>
@@ -11364,10 +11438,19 @@
           <t>Module Tiêu hóa</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr"/>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+![image](note_Câu 444_1750954801.png)</t>
+        </is>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr"/>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Tá tràng</t>
+        </is>
+      </c>
       <c r="B31" t="inlineStr">
         <is>
           <t>Câu 445</t>
@@ -11388,7 +11471,13 @@
           <t>Module Tiêu hóa</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+![image](note_Câu 445_1750954948.png)
+![image](note_Câu 445_1750955077.png)</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr"/>

</xml_diff>